<commit_message>
init module + main flowchart
implemented initializing data step, also implemented main flowchart in performer module
</commit_message>
<xml_diff>
--- a/invoices-processor/performer/du/data/processed/1.jpg.xlsx
+++ b/invoices-processor/performer/du/data/processed/1.jpg.xlsx
@@ -7,7 +7,6 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Simple Fields" sheetId="2" r:id="rId2"/>
-    <x:sheet name="Simple Fields - Formatted" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <x:si>
     <x:t>Invoice Number</x:t>
   </x:si>
@@ -39,9 +38,6 @@
   </x:si>
   <x:si>
     <x:t>$17,310.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17310.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -433,52 +429,4 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
 </file>
</xml_diff>